<commit_message>
Test unit print 4
</commit_message>
<xml_diff>
--- a/public/test_data_pi.xlsx
+++ b/public/test_data_pi.xlsx
@@ -5,16 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="thông tin nhân viên" sheetId="1" r:id="rId1"/>
     <sheet name="thông tin bằng cấp" sheetId="3" r:id="rId2"/>
     <sheet name="thông tin học hàm" sheetId="4" r:id="rId3"/>
+    <sheet name="Thông tin địa chỉ" sheetId="5" r:id="rId4"/>
+    <sheet name="Ghi chú" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="128">
   <si>
     <t>Mã NV</t>
   </si>
@@ -190,9 +192,6 @@
     <t xml:space="preserve">Giảng viên cao cấp </t>
   </si>
   <si>
-    <t>Không</t>
-  </si>
-  <si>
     <t>An GIang</t>
   </si>
   <si>
@@ -289,9 +288,6 @@
     <t xml:space="preserve">  Kinh</t>
   </si>
   <si>
-    <t>Quan hệ công chúng</t>
-  </si>
-  <si>
     <t>kinh</t>
   </si>
   <si>
@@ -337,10 +333,6 @@
     <t>Chuyên khoa Y cấp II</t>
   </si>
   <si>
-    <t>Nước cấp bằng 
-( ghi tên viết tắt )</t>
-  </si>
-  <si>
     <t>vn</t>
   </si>
   <si>
@@ -360,13 +352,73 @@
   </si>
   <si>
     <t>Phó Giáo Sư</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Pr</t>
+  </si>
+  <si>
+    <t>pr</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nước cấp bằng </t>
+  </si>
+  <si>
+    <t>Địa chỉ thường trú</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Địa chỉ </t>
+  </si>
+  <si>
+    <t>Xã phường</t>
+  </si>
+  <si>
+    <t>Quận huyện</t>
+  </si>
+  <si>
+    <t>Tỉnh thành</t>
+  </si>
+  <si>
+    <t>Tôn giáo</t>
+  </si>
+  <si>
+    <t>Phật giáo</t>
+  </si>
+  <si>
+    <t>Hòa hảo</t>
+  </si>
+  <si>
+    <t>Trung An</t>
+  </si>
+  <si>
+    <t>Mỹ thới</t>
+  </si>
+  <si>
+    <t>Long Xuyên</t>
+  </si>
+  <si>
+    <t>Mỹ quý</t>
+  </si>
+  <si>
+    <t>Địa chỉ tạm trú ( liên lạc )</t>
+  </si>
+  <si>
+    <t>Trung An 1</t>
+  </si>
+  <si>
+    <t>Trung An 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +435,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -403,7 +464,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -411,12 +472,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -425,31 +501,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -769,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,8 +869,9 @@
     <col min="5" max="5" width="14" style="3" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
     <col min="12" max="12" width="25.5703125" style="4" customWidth="1"/>
     <col min="13" max="13" width="23.85546875" customWidth="1"/>
     <col min="14" max="14" width="26.7109375" customWidth="1"/>
@@ -794,82 +884,83 @@
     <col min="22" max="22" width="18.85546875" customWidth="1"/>
     <col min="23" max="23" width="20.7109375" customWidth="1"/>
     <col min="24" max="24" width="19.42578125" customWidth="1"/>
+    <col min="25" max="25" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:25" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="W1" s="6" t="s">
+      <c r="V1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="W1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="15" t="s">
         <v>48</v>
       </c>
     </row>
@@ -881,7 +972,7 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -908,7 +999,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M2" s="1">
         <v>43200</v>
@@ -917,7 +1008,7 @@
         <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="P2" t="s">
         <v>50</v>
@@ -950,7 +1041,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -958,7 +1049,7 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -970,7 +1061,7 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>27</v>
@@ -994,36 +1085,36 @@
         <v>24</v>
       </c>
       <c r="O3" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="P3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="R3" t="s">
         <v>49</v>
       </c>
       <c r="S3" t="s">
+        <v>56</v>
+      </c>
+      <c r="T3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="W3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
         <v>59</v>
       </c>
-      <c r="B4" t="s">
-        <v>60</v>
-      </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -1032,25 +1123,25 @@
         <v>35560</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I4" s="1">
         <v>42104</v>
       </c>
       <c r="J4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="M4" s="1">
         <v>43200</v>
@@ -1059,33 +1150,33 @@
         <v>24</v>
       </c>
       <c r="O4" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="P4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q4" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="S4" t="s">
         <v>52</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V4" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="W4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
         <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -1097,25 +1188,25 @@
         <v>35560</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I5" s="1">
         <v>42104</v>
       </c>
       <c r="J5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M5" s="1">
         <v>43200</v>
@@ -1124,31 +1215,28 @@
         <v>24</v>
       </c>
       <c r="O5" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="P5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S5" t="s">
         <v>52</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="U5" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="V5" s="1"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" t="s">
         <v>74</v>
-      </c>
-      <c r="B6" t="s">
-        <v>75</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -1160,25 +1248,25 @@
         <v>35560</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I6" s="1">
         <v>42104</v>
       </c>
       <c r="J6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M6" s="1">
         <v>43200</v>
@@ -1187,19 +1275,19 @@
         <v>24</v>
       </c>
       <c r="O6" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="P6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S6" t="s">
         <v>52</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U6" t="s">
         <v>49</v>
@@ -1210,10 +1298,10 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
         <v>80</v>
-      </c>
-      <c r="B7" t="s">
-        <v>81</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -1225,25 +1313,25 @@
         <v>35560</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I7" s="1">
         <v>42104</v>
       </c>
       <c r="J7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M7" s="1">
         <v>43200</v>
@@ -1252,25 +1340,34 @@
         <v>24</v>
       </c>
       <c r="O7" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="P7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>79</v>
+        <v>66</v>
+      </c>
+      <c r="R7" t="s">
+        <v>49</v>
       </c>
       <c r="S7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U7" t="s">
         <v>49</v>
       </c>
       <c r="V7" s="1">
         <v>43479</v>
+      </c>
+      <c r="W7" t="s">
+        <v>49</v>
+      </c>
+      <c r="X7" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1292,7 +1389,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,212 +1403,212 @@
     <col min="8" max="8" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>94</v>
+      <c r="H1" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="15">
+      <c r="C2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="7">
         <v>43200</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="G2" s="14" t="s">
+      <c r="E2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>96</v>
+      <c r="H2" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="7">
         <v>43441</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="7">
         <v>43388</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="14" t="s">
+      <c r="E4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>98</v>
+      <c r="H4" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="7">
         <v>43388</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G5" s="14" t="s">
+      <c r="E5" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>99</v>
+      <c r="H5" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="7">
         <v>43388</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="14" t="s">
+      <c r="E6" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>100</v>
+      <c r="H6" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="7">
         <v>43388</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G7" s="14" t="s">
+      <c r="E7" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>99</v>
+      <c r="H7" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="7">
+        <v>43388</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="15">
-        <v>43388</v>
-      </c>
-      <c r="E8" s="14" t="s">
+      <c r="G8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1525,7 +1622,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,20 +1633,20 @@
     <col min="5" max="5" width="42.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1558,7 +1655,7 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
@@ -1575,10 +1672,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="1">
         <v>43509</v>
@@ -1590,4 +1687,163 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Unit test Sprint 5
</commit_message>
<xml_diff>
--- a/public/test_data_pi.xlsx
+++ b/public/test_data_pi.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="thông tin nhân viên" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="133">
   <si>
     <t>Mã NV</t>
   </si>
@@ -412,6 +412,21 @@
   </si>
   <si>
     <t>Trung An 2</t>
+  </si>
+  <si>
+    <t>Trưởng phòng</t>
+  </si>
+  <si>
+    <t>Trưởng Khoa</t>
+  </si>
+  <si>
+    <t>Phó trưởng phòng</t>
+  </si>
+  <si>
+    <t>dsadsa</t>
+  </si>
+  <si>
+    <t>Loại cán sự</t>
   </si>
 </sst>
 </file>
@@ -492,7 +507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -504,12 +519,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -540,6 +549,15 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -856,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,86 +903,90 @@
     <col min="23" max="23" width="20.7109375" customWidth="1"/>
     <col min="24" max="24" width="19.42578125" customWidth="1"/>
     <col min="25" max="25" width="12.85546875" customWidth="1"/>
+    <col min="26" max="26" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:26" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="T1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="W1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="X1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Y1" s="13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1040,8 +1062,11 @@
       <c r="Y2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="Z2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1106,7 +1131,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1171,7 +1196,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1230,8 +1255,11 @@
         <v>72</v>
       </c>
       <c r="V5" s="1"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -1295,8 +1323,11 @@
       <c r="V6" s="1">
         <v>43479</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1368,6 +1399,9 @@
       </c>
       <c r="X7" t="s">
         <v>49</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1389,7 +1423,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,28 +1438,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1634,19 +1668,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1693,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,50 +1746,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="9" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1770,7 +1804,7 @@
         <v>126</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
         <v>123</v>

</xml_diff>